<commit_message>
Make DOB into a proper date format (#19)
</commit_message>
<xml_diff>
--- a/etl2/docs/mapping_doc.xlsx
+++ b/etl2/docs/mapping_doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/MOJ/opg-data-casrec-migration/etl2/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B31E55-392B-BA41-B31B-196873E26B08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F348669-41EE-B74E-B4E3-FB7CC90BC9DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22920" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22940" yWindow="460" windowWidth="45860" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="persons (Client)" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="306">
   <si>
     <t>column_name</t>
   </si>
@@ -1023,6 +1023,9 @@
   </si>
   <si>
     <t>Logdate</t>
+  </si>
+  <si>
+    <t>date_format_standard</t>
   </si>
 </sst>
 </file>
@@ -1380,9 +1383,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U19" sqref="U19"/>
+      <selection pane="bottomLeft" activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1531,6 +1534,9 @@
       </c>
       <c r="O5" s="6" t="s">
         <v>25</v>
+      </c>
+      <c r="T5" s="6" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="14" x14ac:dyDescent="0.15">

</xml_diff>